<commit_message>
Adcionado scripts DML E DQL
</commit_message>
<xml_diff>
--- a/Exercicios/Exercicio 1.2 locadora/Modelo/Locadora Exercicio 1.2 Fisico.xlsx
+++ b/Exercicios/Exercicio 1.2 locadora/Modelo/Locadora Exercicio 1.2 Fisico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sprint 1 Bd\Senai_sprint1_bd\Exercicios\Exercicio 1.2 locadora\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sprint 1 Bd\Senai_sprint1_bd\Exercicios\Exercicio 1.2 locadora\Modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE968D1E-8FD0-431D-BE7C-942BE66A9309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71382C03-35DD-44AE-A57D-E287FB2B1A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{77F0E013-A4B6-4EAC-A888-22D44FB664B1}"/>
+    <workbookView xWindow="5355" yWindow="690" windowWidth="15375" windowHeight="8325" xr2:uid="{77F0E013-A4B6-4EAC-A888-22D44FB664B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2388D7-DE52-4B04-965C-D2ECE9F319F0}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adcionado exercicios de SELECT JOIN no DQL
</commit_message>
<xml_diff>
--- a/Exercicios/Exercicio 1.2 locadora/Modelo/Locadora Exercicio 1.2 Fisico.xlsx
+++ b/Exercicios/Exercicio 1.2 locadora/Modelo/Locadora Exercicio 1.2 Fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sprint 1 Bd\Senai_sprint1_bd\Exercicios\Exercicio 1.2 locadora\Modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71382C03-35DD-44AE-A57D-E287FB2B1A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D15727-EC54-4E0D-AA42-CDD257E647AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="690" windowWidth="15375" windowHeight="8325" xr2:uid="{77F0E013-A4B6-4EAC-A888-22D44FB664B1}"/>
+    <workbookView xWindow="2970" yWindow="1560" windowWidth="15375" windowHeight="8325" xr2:uid="{77F0E013-A4B6-4EAC-A888-22D44FB664B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Veiculos</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>8K0</t>
+  </si>
+  <si>
+    <t>DataEmissão</t>
+  </si>
+  <si>
+    <t>DataDevolução</t>
   </si>
 </sst>
 </file>
@@ -159,8 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2388D7-DE52-4B04-965C-D2ECE9F319F0}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,9 +497,11 @@
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -529,7 +538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -581,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -601,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -612,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -637,8 +646,14 @@
       <c r="M14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -663,8 +678,14 @@
       <c r="M15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1">
+        <v>44413</v>
+      </c>
+      <c r="O15" s="1">
+        <v>44423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -683,8 +704,14 @@
       <c r="M16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1">
+        <v>44423</v>
+      </c>
+      <c r="O16" s="1">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K17">
         <v>3</v>
       </c>
@@ -693,6 +720,12 @@
       </c>
       <c r="M17">
         <v>3</v>
+      </c>
+      <c r="N17" s="1">
+        <v>44414</v>
+      </c>
+      <c r="O17" s="1">
+        <v>44418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>